<commit_message>
Agregamos los listados del 22 de julio de 2024
</commit_message>
<xml_diff>
--- a/Julio/22 julio/chontalpa/PLANTILLA LISTA DE ASPIRANTES_1 (9).xlsx
+++ b/Julio/22 julio/chontalpa/PLANTILLA LISTA DE ASPIRANTES_1 (9).xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Centro de Computo\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MaxoC\OneDrive\Documents\EVALUATEC2024\Julio\22 julio\chontalpa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{373135C1-73C8-4566-9621-976E2C2758C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F87F7216-FD1C-4682-91AA-05B4C9C4E520}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D610CFFB-2790-104B-A52B-2B33694C28D9}"/>
   </bookViews>
@@ -396,17 +396,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -450,6 +450,9 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{5925BC7A-0E73-734D-A0C9-B8A68F88FF64}" name="Tabla2" displayName="Tabla2" ref="A4:M21" totalsRowShown="0">
   <autoFilter ref="A4:M21" xr:uid="{5925BC7A-0E73-734D-A0C9-B8A68F88FF64}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:M21">
+    <sortCondition ref="F4:F21"/>
+  </sortState>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{F5111305-CA2B-DF41-BA05-5C9A177B7523}" name="FICHA"/>
     <tableColumn id="2" xr3:uid="{D956ADB6-2882-CB4B-9C6B-032AC358A5C1}" name="NOMBRE ASPIRANTE"/>
@@ -769,7 +772,7 @@
   <dimension ref="A1:M21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -778,9 +781,9 @@
     <col min="2" max="2" width="21" customWidth="1"/>
     <col min="3" max="3" width="21.25" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.5" customWidth="1"/>
-    <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.75" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33.25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.375" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="16.125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="22.375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="21.875" bestFit="1" customWidth="1"/>
@@ -789,23 +792,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="41.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="L1" s="10"/>
+      <c r="L1" s="9"/>
     </row>
     <row r="2" spans="1:13" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="L2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+      <c r="L2" s="9"/>
     </row>
     <row r="3" spans="1:13" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="L3" s="10"/>
+      <c r="L3" s="9"/>
     </row>
     <row r="4" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -850,143 +853,143 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>83</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>84</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>18</v>
+        <v>85</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>87</v>
       </c>
       <c r="F5" t="s">
-        <v>19</v>
+        <v>88</v>
       </c>
       <c r="G5" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="6"/>
-      <c r="I5" s="7"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="6"/>
       <c r="J5" s="1">
         <v>45495</v>
       </c>
       <c r="K5" s="2">
         <v>0.45833333333333331</v>
       </c>
-      <c r="L5" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="M5" s="7"/>
+      <c r="L5" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="M5" s="6"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>49</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>50</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>24</v>
+        <v>51</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>53</v>
       </c>
       <c r="F6" t="s">
-        <v>25</v>
+        <v>54</v>
       </c>
       <c r="G6" t="s">
         <v>10</v>
       </c>
-      <c r="H6" s="6"/>
-      <c r="I6" s="7"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="6"/>
       <c r="J6" s="1">
         <v>45495</v>
       </c>
       <c r="K6" s="2">
         <v>0.45833333333333331</v>
       </c>
-      <c r="L6" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="M6" s="7"/>
+      <c r="L6" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="M6" s="6"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>55</v>
       </c>
       <c r="B7" t="s">
-        <v>27</v>
+        <v>56</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>24</v>
+        <v>57</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>53</v>
       </c>
       <c r="F7" t="s">
-        <v>25</v>
+        <v>54</v>
       </c>
       <c r="G7" t="s">
         <v>10</v>
       </c>
-      <c r="H7" s="6"/>
-      <c r="I7" s="7"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="6"/>
       <c r="J7" s="1">
         <v>45495</v>
       </c>
       <c r="K7" s="2">
         <v>0.45833333333333331</v>
       </c>
-      <c r="L7" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="M7" s="7"/>
+      <c r="L7" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="M7" s="6"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>28</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>24</v>
+        <v>16</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="F8" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="G8" t="s">
         <v>10</v>
       </c>
-      <c r="H8" s="6"/>
-      <c r="I8" s="7"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="6"/>
       <c r="J8" s="1">
         <v>45495</v>
       </c>
       <c r="K8" s="2">
         <v>0.45833333333333331</v>
       </c>
-      <c r="L8" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="M8" s="7"/>
+      <c r="L8" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="M8" s="6"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -998,10 +1001,10 @@
       <c r="C9" t="s">
         <v>34</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="D9" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="E9" s="9" t="s">
+      <c r="E9" s="8" t="s">
         <v>18</v>
       </c>
       <c r="F9" t="s">
@@ -1010,18 +1013,18 @@
       <c r="G9" t="s">
         <v>10</v>
       </c>
-      <c r="H9" s="6"/>
-      <c r="I9" s="7"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="6"/>
       <c r="J9" s="1">
         <v>45495</v>
       </c>
       <c r="K9" s="2">
         <v>0.45833333333333331</v>
       </c>
-      <c r="L9" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="M9" s="7"/>
+      <c r="L9" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="M9" s="6"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -1033,10 +1036,10 @@
       <c r="C10" t="s">
         <v>38</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="D10" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="E10" s="9" t="s">
+      <c r="E10" s="8" t="s">
         <v>18</v>
       </c>
       <c r="F10" t="s">
@@ -1045,68 +1048,68 @@
       <c r="G10" t="s">
         <v>10</v>
       </c>
-      <c r="H10" s="6"/>
-      <c r="I10" s="7"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="6"/>
       <c r="J10" s="1">
         <v>45495</v>
       </c>
       <c r="K10" s="2">
         <v>0.45833333333333331</v>
       </c>
-      <c r="L10" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="M10" s="7"/>
+      <c r="L10" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="M10" s="6"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B11" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C11" t="s">
-        <v>42</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="E11" s="9" t="s">
-        <v>24</v>
+        <v>46</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="F11" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="G11" t="s">
         <v>10</v>
       </c>
-      <c r="H11" s="6"/>
-      <c r="I11" s="7"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="6"/>
       <c r="J11" s="1">
         <v>45495</v>
       </c>
       <c r="K11" s="2">
         <v>0.45833333333333331</v>
       </c>
-      <c r="L11" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="M11" s="7"/>
+      <c r="L11" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="M11" s="6"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="B12" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="C12" t="s">
-        <v>46</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="E12" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="E12" s="8" t="s">
         <v>18</v>
       </c>
       <c r="F12" t="s">
@@ -1115,138 +1118,138 @@
       <c r="G12" t="s">
         <v>10</v>
       </c>
-      <c r="H12" s="6"/>
-      <c r="I12" s="7"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="6"/>
       <c r="J12" s="1">
         <v>45495</v>
       </c>
       <c r="K12" s="2">
         <v>0.45833333333333331</v>
       </c>
-      <c r="L12" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="M12" s="7"/>
+      <c r="L12" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="M12" s="6"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>49</v>
+        <v>79</v>
       </c>
       <c r="B13" t="s">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="C13" t="s">
-        <v>51</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="E13" s="9" t="s">
-        <v>53</v>
+        <v>81</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="F13" t="s">
-        <v>54</v>
+        <v>19</v>
       </c>
       <c r="G13" t="s">
         <v>10</v>
       </c>
-      <c r="H13" s="6"/>
-      <c r="I13" s="7"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="6"/>
       <c r="J13" s="1">
         <v>45495</v>
       </c>
       <c r="K13" s="2">
         <v>0.45833333333333331</v>
       </c>
-      <c r="L13" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="M13" s="7"/>
+      <c r="L13" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="M13" s="6"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>55</v>
+        <v>20</v>
       </c>
       <c r="B14" t="s">
-        <v>56</v>
+        <v>21</v>
       </c>
       <c r="C14" t="s">
-        <v>57</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="E14" s="9" t="s">
-        <v>53</v>
+        <v>22</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>24</v>
       </c>
       <c r="F14" t="s">
-        <v>54</v>
+        <v>25</v>
       </c>
       <c r="G14" t="s">
         <v>10</v>
       </c>
-      <c r="H14" s="6"/>
-      <c r="I14" s="7"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="6"/>
       <c r="J14" s="1">
         <v>45495</v>
       </c>
       <c r="K14" s="2">
         <v>0.45833333333333331</v>
       </c>
-      <c r="L14" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="M14" s="7"/>
+      <c r="L14" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="M14" s="6"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
       <c r="B15" t="s">
-        <v>60</v>
+        <v>27</v>
       </c>
       <c r="C15" t="s">
-        <v>61</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="E15" s="9" t="s">
-        <v>18</v>
+        <v>28</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>24</v>
       </c>
       <c r="F15" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="G15" t="s">
         <v>10</v>
       </c>
-      <c r="H15" s="6"/>
-      <c r="I15" s="7"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="6"/>
       <c r="J15" s="1">
         <v>45495</v>
       </c>
       <c r="K15" s="2">
         <v>0.45833333333333331</v>
       </c>
-      <c r="L15" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="M15" s="7"/>
+      <c r="L15" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="M15" s="6"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>63</v>
+        <v>30</v>
       </c>
       <c r="B16" t="s">
-        <v>64</v>
+        <v>27</v>
       </c>
       <c r="C16" t="s">
-        <v>65</v>
-      </c>
-      <c r="D16" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="E16" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E16" s="8" t="s">
         <v>24</v>
       </c>
       <c r="F16" t="s">
@@ -1255,33 +1258,33 @@
       <c r="G16" t="s">
         <v>10</v>
       </c>
-      <c r="H16" s="6"/>
-      <c r="I16" s="7"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="6"/>
       <c r="J16" s="1">
         <v>45495</v>
       </c>
       <c r="K16" s="2">
         <v>0.45833333333333331</v>
       </c>
-      <c r="L16" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="M16" s="7"/>
+      <c r="L16" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="M16" s="6"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>67</v>
+        <v>40</v>
       </c>
       <c r="B17" t="s">
-        <v>68</v>
+        <v>41</v>
       </c>
       <c r="C17" t="s">
-        <v>69</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="E17" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="E17" s="8" t="s">
         <v>24</v>
       </c>
       <c r="F17" t="s">
@@ -1290,33 +1293,33 @@
       <c r="G17" t="s">
         <v>10</v>
       </c>
-      <c r="H17" s="6"/>
-      <c r="I17" s="7"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="6"/>
       <c r="J17" s="1">
         <v>45495</v>
       </c>
       <c r="K17" s="2">
         <v>0.45833333333333331</v>
       </c>
-      <c r="L17" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="M17" s="7"/>
+      <c r="L17" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="M17" s="6"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="B18" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C18" t="s">
-        <v>73</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="E18" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="E18" s="8" t="s">
         <v>24</v>
       </c>
       <c r="F18" t="s">
@@ -1325,33 +1328,33 @@
       <c r="G18" t="s">
         <v>10</v>
       </c>
-      <c r="H18" s="6"/>
-      <c r="I18" s="7"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="6"/>
       <c r="J18" s="1">
         <v>45495</v>
       </c>
       <c r="K18" s="2">
         <v>0.45833333333333331</v>
       </c>
-      <c r="L18" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="M18" s="7"/>
+      <c r="L18" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="M18" s="6"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="B19" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="C19" t="s">
-        <v>77</v>
-      </c>
-      <c r="D19" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="E19" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="E19" s="8" t="s">
         <v>24</v>
       </c>
       <c r="F19" t="s">
@@ -1360,88 +1363,88 @@
       <c r="G19" t="s">
         <v>10</v>
       </c>
-      <c r="H19" s="6"/>
-      <c r="I19" s="7"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="6"/>
       <c r="J19" s="1">
         <v>45495</v>
       </c>
       <c r="K19" s="2">
         <v>0.45833333333333331</v>
       </c>
-      <c r="L19" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="M19" s="7"/>
+      <c r="L19" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="M19" s="6"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="B20" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="C20" t="s">
-        <v>81</v>
-      </c>
-      <c r="D20" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="E20" s="9" t="s">
-        <v>18</v>
+        <v>73</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>24</v>
       </c>
       <c r="F20" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="G20" t="s">
         <v>10</v>
       </c>
-      <c r="H20" s="6"/>
-      <c r="I20" s="7"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="6"/>
       <c r="J20" s="1">
         <v>45495</v>
       </c>
       <c r="K20" s="2">
         <v>0.45833333333333331</v>
       </c>
-      <c r="L20" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="M20" s="7"/>
+      <c r="L20" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="M20" s="6"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="B21" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="C21" t="s">
-        <v>85</v>
-      </c>
-      <c r="D21" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="E21" s="9" t="s">
-        <v>87</v>
+        <v>77</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>24</v>
       </c>
       <c r="F21" t="s">
-        <v>88</v>
+        <v>25</v>
       </c>
       <c r="G21" t="s">
         <v>10</v>
       </c>
-      <c r="H21" s="6"/>
-      <c r="I21" s="7"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="6"/>
       <c r="J21" s="1">
         <v>45495</v>
       </c>
       <c r="K21" s="2">
         <v>0.45833333333333331</v>
       </c>
-      <c r="L21" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="M21" s="7"/>
+      <c r="L21" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="M21" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>